<commit_message>
Se eliminaron los archivos .xlsx por pais. Se agregó base de datos por región. La línea de predicción la hice más gruesa, porque no se veía nada antes. Reporte del día 22 para países
</commit_message>
<xml_diff>
--- a/casos_pais.xlsx
+++ b/casos_pais.xlsx
@@ -141,8 +141,8 @@
   </sheetPr>
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -796,6 +796,18 @@
       <c r="B37" s="0" t="n">
         <v>36</v>
       </c>
+      <c r="C37" s="0" t="n">
+        <v>632</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>1178</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>25496</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>53578</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">

</xml_diff>